<commit_message>
v1.4.0.0 alpha. Implements ForeignInfoColumns. Fixing first standard version.
</commit_message>
<xml_diff>
--- a/AIWE Table Making Guideline 20180228.xlsx
+++ b/AIWE Table Making Guideline 20180228.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Common Tables" sheetId="1" r:id="rId1"/>
@@ -5471,10 +5471,31 @@
     <t>N'PrefilledColumns;ItemsPerPage;OrderBy;ActionList;DefaultActionList;TableActionList;DefaultTableActionList;TextFieldColumns;PictureColumns;IndexShownPictureColumns;RequiredColumns;NumberLimitColumns;RegexCheckedColumns;RegexCheckedColumnExamples;UserRelatedFilters;DisableFilter;ForcedFilterColumns;ColumnExclusionList;FilterExclusionList;DetailsExclusionList;CreateEditExclusionList;CsvExclusionList;AccessExclusionList;ColoringList;FilterDropDownLists;CreateEditDropDownLists;PrefixesOfColumns;PostfixesOfColumns;ListColumns;TimeStampColumns;HistoryTable;HistoryTrigger;AutoGeneratedColumns;ColumnSequence;ColumnAliases;EditShowOnlyColumns;ScriptConstructorColumns;ScriptColumns;CustomDateTimeFormatColumns;EmailMakerTriggers;EmailMakers;NonPictureAttachmentColumns;DownloadColumns;PreActionTriggers;PreActionProcedures;PostActionTriggers;PostActionProcedures;AggregationStatement;ForeignInfoColumns', --ColumnExclusionList</t>
   </si>
   <si>
+    <t>ColumnName1=RefTableName1:ForeignKeyColumnName1;
+ColumnName2=RefTableName2:ForeignKeyColumnName2:RefColumnName21,RefColumnName22,…,RefColumnName2N;
+ColumnName3=RefTableName3:ForeignKeyColumnName3:RefColumnName31|RefColumnDisplayName31,RefColumnName32|RefColumnDisplayName32,…,RefColumnName3N|RefColumnDisplayName3N;</t>
+  </si>
+  <si>
+    <t>Example: ProductId=TBL_PRODUCT_DESC:Id:ProductCode,ProductType,ProductDesc|Display Differently
+Means:
+- The ProductId column is a foreign key to TBL_PRODUCT_DESC table, Id column.
+- Takes ProductCode, ProductType, and ProductDesc column values from TBL_PRODUCT_DESC to be displayed.
+- ProductCode and ProductType are displayed as "Product Code" and "Product Type" respectively. But ProductDesc is displayed as "Displayed Differently"</t>
+  </si>
+  <si>
+    <t>Row action list of the named table, applied to every row of the table entries, except for Create and CreateGroup.
+Currently available default row actions: Create, Edit, Delete, Details, DownloadAttachments, CreateGroup, DeleteGroup, GroupDetails.
+CreateGroup, EditGroup, DeleteGroup, and GroupDetails are only applicable for [Group] [TableType].
+  Any customized row action will be applied to individual item, not to a group, even when [TableType] is [Group]
+Role is used to specify user roles to whom this column criteria will be applied
+[Developer] and [Main Administrator] roles are immune from role restrictions</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">To specify columns which represent foreign keys to other table's columns and to display (not to edit or to delete) the other table's data columns. If not specified, all other table's column data will be displayed except the foreign key column value itself. 
 To select some other table's data columns to be displayed, specify the RefColumnName(s) of the other table's columns. 
 To display the RefColumnName(s) differently than how the column names are defined in the database, specify the RefColumnDisplayName(s). If the RefColumnDisplayName(s) is(are) not specified, default RefColumnName(s) will be assumed. 
+For AIWE: only applied for [Dropdown Columns].
 </t>
     </r>
     <r>
@@ -5498,26 +5519,6 @@
       </rPr>
       <t>: do not use symbols (such as : , ? | etc) as RefColumnDisplayName(s) components.</t>
     </r>
-  </si>
-  <si>
-    <t>ColumnName1=RefTableName1:ForeignKeyColumnName1;
-ColumnName2=RefTableName2:ForeignKeyColumnName2:RefColumnName21,RefColumnName22,…,RefColumnName2N;
-ColumnName3=RefTableName3:ForeignKeyColumnName3:RefColumnName31|RefColumnDisplayName31,RefColumnName32|RefColumnDisplayName32,…,RefColumnName3N|RefColumnDisplayName3N;</t>
-  </si>
-  <si>
-    <t>Example: ProductId=TBL_PRODUCT_DESC:Id:ProductCode,ProductType,ProductDesc|Display Differently
-Means:
-- The ProductId column is a foreign key to TBL_PRODUCT_DESC table, Id column.
-- Takes ProductCode, ProductType, and ProductDesc column values from TBL_PRODUCT_DESC to be displayed.
-- ProductCode and ProductType are displayed as "Product Code" and "Product Type" respectively. But ProductDesc is displayed as "Displayed Differently"</t>
-  </si>
-  <si>
-    <t>Row action list of the named table, applied to every row of the table entries, except for Create and CreateGroup.
-Currently available default row actions: Create, Edit, Delete, Details, DownloadAttachments, CreateGroup, DeleteGroup, GroupDetails.
-CreateGroup, EditGroup, DeleteGroup, and GroupDetails are only applicable for [Group] [TableType].
-  Any customized row action will be applied to individual item, not to a group, even when [TableType] is [Group]
-Role is used to specify user roles to whom this column criteria will be applied
-[Developer] and [Main Administrator] roles are immune from role restrictions</t>
   </si>
 </sst>
 </file>
@@ -6309,7 +6310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
@@ -10734,8 +10735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10898,7 +10899,7 @@
         <v>168</v>
       </c>
       <c r="E9" s="83" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="F9" s="34"/>
     </row>
@@ -11758,7 +11759,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="82" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" s="82" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A55" s="81">
         <v>53</v>
       </c>
@@ -11769,13 +11770,13 @@
         <v>1170</v>
       </c>
       <c r="D55" s="53" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E55" s="53" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F55" s="53" t="s">
         <v>1182</v>
-      </c>
-      <c r="E55" s="53" t="s">
-        <v>1181</v>
-      </c>
-      <c r="F55" s="53" t="s">
-        <v>1183</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>